<commit_message>
created function: 'imalign' and test-script: 'rotation
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18528"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -439,7 +439,7 @@
   <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -450,7 +450,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1">
-        <v>1</v>
+        <v>80</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -462,7 +462,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>2</v>
+        <v>81</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>1</v>
@@ -474,7 +474,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>3</v>
+        <v>82</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>2</v>
@@ -486,7 +486,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>4</v>
+        <v>83</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>3</v>
@@ -498,7 +498,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>5</v>
+        <v>84</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>4</v>
@@ -510,7 +510,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>6</v>
+        <v>85</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>5</v>
@@ -522,7 +522,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>7</v>
+        <v>86</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>6</v>
@@ -534,7 +534,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>8</v>
+        <v>87</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>7</v>
@@ -546,7 +546,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>9</v>
+        <v>88</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>8</v>
@@ -558,7 +558,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>10</v>
+        <v>89</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>9</v>
@@ -570,7 +570,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>11</v>
+        <v>90</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>10</v>
@@ -582,7 +582,7 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>12</v>
+        <v>91</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>11</v>
@@ -594,7 +594,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>13</v>
+        <v>92</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>12</v>
@@ -606,7 +606,7 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>14</v>
+        <v>93</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>13</v>
@@ -618,7 +618,7 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>15</v>
+        <v>94</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>14</v>
@@ -630,7 +630,7 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>16</v>
+        <v>95</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>15</v>
@@ -642,7 +642,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>17</v>
+        <v>96</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>16</v>
@@ -654,7 +654,7 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>18</v>
+        <v>97</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>17</v>
@@ -666,7 +666,7 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>19</v>
+        <v>98</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>18</v>
@@ -678,7 +678,7 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>20</v>
+        <v>99</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>19</v>

</xml_diff>